<commit_message>
Fixed FP.2 and matchBoundingBoxes
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JonghwanShin/Sources/SFND_3D_Object_Tracking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FE8E13-0A63-4042-9D62-5F663962C0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05577B73-35F3-B64A-9C53-ACBF6A18E233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-67160" yWindow="7200" windowWidth="68800" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2540" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Processed" sheetId="2" r:id="rId1"/>
@@ -198,7 +198,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -332,6 +332,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -675,8 +681,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3833,46 +3841,6 @@
           <c:yVal>
             <c:numRef>
               <c:f>Processed!$AE$2:$AE$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>12.370377</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16.141013999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15.445668</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.833313</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11.79195</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12.271898</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>11.349665</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10.378202</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10.654106000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10.064767</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.4629580000000004</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9.0772700000000004</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
@@ -3974,6 +3942,46 @@
           <c:yVal>
             <c:numRef>
               <c:f>Processed!$AF$2:$AF$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>12.098753</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.616270999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.811176</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.612500000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.311249</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.128569000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.187908</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9263949999999994</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.124207999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0901990000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.9464790000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.9160660000000007</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
@@ -4462,40 +4470,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>12.515599999999999</c:v>
+                  <c:v>12.289099999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.908232999999999</c:v>
+                  <c:v>12.729945000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.984351</c:v>
+                  <c:v>13.731432</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.124117999999999</c:v>
+                  <c:v>13.790126000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.174640999999999</c:v>
+                  <c:v>11.864185000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.808600999999999</c:v>
+                  <c:v>11.968197</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.9597800000000003</c:v>
+                  <c:v>9.8871129999999994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.59863</c:v>
+                  <c:v>9.3021480000000007</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.5735250000000001</c:v>
+                  <c:v>8.3211999999999993</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.5161700000000007</c:v>
+                  <c:v>8.8986730000000005</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.5465809999999998</c:v>
+                  <c:v>11.030113999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.3988029999999991</c:v>
+                  <c:v>8.5355679999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5282,16 +5290,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>52</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5616,10 +5624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ45"/>
+  <dimension ref="A1:AK45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG12" sqref="AG12"/>
+      <selection activeCell="AM6" sqref="AM6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5627,16 +5635,12 @@
     <col min="2" max="2" width="18.6640625" hidden="1" customWidth="1"/>
     <col min="3" max="5" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="6" max="8" width="13" hidden="1" customWidth="1"/>
-    <col min="9" max="12" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="13" max="14" width="0" hidden="1" customWidth="1"/>
-    <col min="15" max="30" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="10.83203125" customWidth="1"/>
-    <col min="32" max="32" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="33" max="34" width="10.83203125" customWidth="1"/>
-    <col min="35" max="35" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="31" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="32" max="34" width="10.83203125" customWidth="1"/>
+    <col min="35" max="35" width="10.83203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B1" t="str">
         <f ca="1">CONCATENATE(OFFSET(Raw!$A$2, 12*(COLUMN()-2), 0),"/",OFFSET(Raw!$A$2, 12*(COLUMN()-2), 1))</f>
         <v>SHITOMASI/BRIEF</v>
@@ -5777,7 +5781,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5898,10 +5902,11 @@
         <v>11.619621</v>
       </c>
       <c r="AJ2">
-        <v>12.515599999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+        <v>12.289099999999999</v>
+      </c>
+      <c r="AK2" s="1"/>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6030,10 +6035,11 @@
         <v>13.624651</v>
       </c>
       <c r="AJ3">
-        <v>15.908232999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+        <v>12.729945000000001</v>
+      </c>
+      <c r="AK3" s="1"/>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6166,10 +6172,11 @@
         <v>14.842502</v>
       </c>
       <c r="AJ4">
-        <v>11.984351</v>
-      </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+        <v>13.731432</v>
+      </c>
+      <c r="AK4" s="1"/>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6310,10 +6317,11 @@
         <v>11.32192</v>
       </c>
       <c r="AJ5">
-        <v>13.124117999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+        <v>13.790126000000001</v>
+      </c>
+      <c r="AK5" s="1"/>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6454,10 +6462,11 @@
         <v>11.336739</v>
       </c>
       <c r="AJ6">
-        <v>11.174640999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+        <v>11.864185000000001</v>
+      </c>
+      <c r="AK6" s="1"/>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6586,10 +6595,11 @@
         <v>11.490812999999999</v>
       </c>
       <c r="AJ7">
-        <v>12.808600999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+        <v>11.968197</v>
+      </c>
+      <c r="AK7" s="1"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6710,10 +6720,11 @@
         <v>10.363201999999999</v>
       </c>
       <c r="AJ8">
-        <v>8.9597800000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+        <v>9.8871129999999994</v>
+      </c>
+      <c r="AK8" s="1"/>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -6838,10 +6849,11 @@
         <v>10.077458999999999</v>
       </c>
       <c r="AJ9">
-        <v>9.59863</v>
-      </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+        <v>9.3021480000000007</v>
+      </c>
+      <c r="AK9" s="1"/>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -6982,10 +6994,11 @@
         <v>9.1397779999999997</v>
       </c>
       <c r="AJ10">
-        <v>8.5735250000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+        <v>8.3211999999999993</v>
+      </c>
+      <c r="AK10" s="1"/>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -7126,10 +7139,11 @@
         <v>8.6510259999999999</v>
       </c>
       <c r="AJ11">
-        <v>9.5161700000000007</v>
-      </c>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+        <v>8.8986730000000005</v>
+      </c>
+      <c r="AK11" s="1"/>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -7258,10 +7272,11 @@
         <v>8.8412349999999993</v>
       </c>
       <c r="AJ12">
-        <v>9.5465809999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+        <v>11.030113999999999</v>
+      </c>
+      <c r="AK12" s="1"/>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -7386,8 +7401,9 @@
         <v>12.2751</v>
       </c>
       <c r="AJ13">
-        <v>8.3988029999999991</v>
-      </c>
+        <v>8.5355679999999996</v>
+      </c>
+      <c r="AK13" s="1"/>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
@@ -7504,139 +7520,139 @@
       </c>
       <c r="B30">
         <f t="shared" ref="B30:AI30" ca="1" si="0">ABS(B2-$AJ2)</f>
-        <v>1.4530740000000009</v>
+        <v>1.6795740000000006</v>
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5589330000000015</v>
+        <v>1.7854330000000012</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0516890000000014</v>
+        <v>1.2781890000000011</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85329300000000075</v>
+        <v>1.0797930000000004</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5591190000000008</v>
+        <v>1.7856190000000005</v>
       </c>
       <c r="G30">
         <f t="shared" si="0"/>
-        <v>12.515599999999999</v>
+        <v>12.289099999999999</v>
       </c>
       <c r="H30">
         <f t="shared" si="0"/>
-        <v>12.515599999999999</v>
+        <v>12.289099999999999</v>
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
-        <v>12.515599999999999</v>
+        <v>12.289099999999999</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>12.515599999999999</v>
+        <v>12.289099999999999</v>
       </c>
       <c r="K30">
         <f t="shared" si="0"/>
-        <v>12.515599999999999</v>
+        <v>12.289099999999999</v>
       </c>
       <c r="L30">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9328999999998615E-2</v>
+        <v>0.18717100000000109</v>
       </c>
       <c r="M30">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0900999999998504E-2</v>
+        <v>0.2055990000000012</v>
       </c>
       <c r="N30">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3780189999999983</v>
+        <v>1.1515189999999986</v>
       </c>
       <c r="O30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54612299999999969</v>
+        <v>0.31962299999999999</v>
       </c>
       <c r="P30">
         <f t="shared" ca="1" si="0"/>
-        <v>9.1515000000001123E-2</v>
+        <v>0.31801500000000082</v>
       </c>
       <c r="Q30">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3819860000000013</v>
+        <v>1.608486000000001</v>
       </c>
       <c r="R30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.65387800000000063</v>
+        <v>0.88037800000000033</v>
       </c>
       <c r="S30">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2672450000000008</v>
+        <v>1.4937450000000005</v>
       </c>
       <c r="T30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17768199999999901</v>
+        <v>4.8818000000000694E-2</v>
       </c>
       <c r="U30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.40586400000000111</v>
+        <v>0.63236400000000081</v>
       </c>
       <c r="V30">
         <f t="shared" ca="1" si="0"/>
-        <v>11.38918</v>
+        <v>11.615679999999999</v>
       </c>
       <c r="W30">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5736950000000007</v>
+        <v>2.8001950000000004</v>
       </c>
       <c r="X30">
         <f t="shared" ca="1" si="0"/>
-        <v>35.722748000000003</v>
+        <v>35.949248000000004</v>
       </c>
       <c r="Y30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33650799999999848</v>
+        <v>0.11000799999999877</v>
       </c>
       <c r="Z30">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5169720000000009</v>
+        <v>2.7434720000000006</v>
       </c>
       <c r="AA30">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1829970000000003</v>
+        <v>1.409497</v>
       </c>
       <c r="AB30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31066000000000038</v>
+        <v>0.53716000000000008</v>
       </c>
       <c r="AC30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48702600000000018</v>
+        <v>0.71352599999999988</v>
       </c>
       <c r="AD30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41621099999999878</v>
+        <v>0.18971099999999907</v>
       </c>
       <c r="AE30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14522299999999966</v>
+        <v>8.1277000000000044E-2</v>
       </c>
       <c r="AF30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41684699999999886</v>
+        <v>0.19034699999999916</v>
       </c>
       <c r="AG30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.92380299999999949</v>
+        <v>0.69730299999999978</v>
       </c>
       <c r="AH30">
         <f t="shared" ca="1" si="0"/>
-        <v>1.216018</v>
+        <v>0.98951800000000034</v>
       </c>
       <c r="AI30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.89597899999999875</v>
+        <v>0.66947899999999905</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.2">
@@ -7645,139 +7661,139 @@
       </c>
       <c r="B31">
         <f t="shared" ref="B31:AI31" ca="1" si="1">ABS(B3-$AJ3)</f>
-        <v>3.7770529999999987</v>
+        <v>0.59876500000000021</v>
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3367290000000001</v>
+        <v>0.15844100000000161</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="1"/>
-        <v>3.6335509999999989</v>
+        <v>0.45526300000000042</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3143549999999991</v>
+        <v>0.1360670000000006</v>
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="1"/>
-        <v>3.465484</v>
+        <v>0.28719600000000156</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
-        <v>15.908232999999999</v>
+        <v>12.729945000000001</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="1"/>
-        <v>306.21448700000002</v>
+        <v>309.39277500000003</v>
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="1"/>
-        <v>9.4410509999999981</v>
+        <v>6.2627630000000005</v>
       </c>
       <c r="J31">
         <f t="shared" ca="1" si="1"/>
-        <v>306.21448700000002</v>
+        <v>309.39277500000003</v>
       </c>
       <c r="K31">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1199629999999985</v>
+        <v>2.941675</v>
       </c>
       <c r="L31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7914519999999996</v>
+        <v>2.3868359999999988</v>
       </c>
       <c r="M31">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2574769999999997</v>
+        <v>0.92081099999999871</v>
       </c>
       <c r="N31">
         <f t="shared" ca="1" si="1"/>
-        <v>2.909103</v>
+        <v>0.26918499999999845</v>
       </c>
       <c r="O31">
         <f t="shared" ca="1" si="1"/>
-        <v>3.6805229999999991</v>
+        <v>0.50223500000000065</v>
       </c>
       <c r="P31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16483399999999904</v>
+        <v>3.0134539999999994</v>
       </c>
       <c r="Q31">
         <f t="shared" ca="1" si="1"/>
-        <v>4.0212260000000022</v>
+        <v>7.1995140000000006</v>
       </c>
       <c r="R31">
         <f t="shared" ca="1" si="1"/>
-        <v>11.789408999999999</v>
+        <v>14.967696999999998</v>
       </c>
       <c r="S31">
         <f t="shared" ca="1" si="1"/>
-        <v>5.7527819999999998</v>
+        <v>8.9310699999999983</v>
       </c>
       <c r="T31">
         <f t="shared" ca="1" si="1"/>
-        <v>7.7475670000000001</v>
+        <v>10.925854999999999</v>
       </c>
       <c r="U31">
         <f t="shared" ca="1" si="1"/>
-        <v>15.963837000000002</v>
+        <v>19.142125</v>
       </c>
       <c r="V31">
         <f t="shared" si="1"/>
-        <v>15.908232999999999</v>
+        <v>12.729945000000001</v>
       </c>
       <c r="W31">
         <f t="shared" ca="1" si="1"/>
-        <v>15.908232999999999</v>
+        <v>12.729945000000001</v>
       </c>
       <c r="X31">
         <f t="shared" ca="1" si="1"/>
-        <v>15.908232999999999</v>
+        <v>12.729945000000001</v>
       </c>
       <c r="Y31">
         <f t="shared" ca="1" si="1"/>
-        <v>15.908232999999999</v>
+        <v>12.729945000000001</v>
       </c>
       <c r="Z31">
         <f t="shared" si="1"/>
-        <v>15.908232999999999</v>
+        <v>12.729945000000001</v>
       </c>
       <c r="AA31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.716448999999999</v>
+        <v>2.4618389999999994</v>
       </c>
       <c r="AB31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.99306699999999992</v>
+        <v>2.1852209999999985</v>
       </c>
       <c r="AC31">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0515000000001393E-2</v>
+        <v>3.1988029999999998</v>
       </c>
       <c r="AD31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4215769999999992</v>
+        <v>3.5998649999999977</v>
       </c>
       <c r="AE31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.23278099999999924</v>
+        <v>3.4110689999999977</v>
       </c>
       <c r="AF31">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2919619999999998</v>
+        <v>0.88632599999999861</v>
       </c>
       <c r="AG31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.79170999999999836</v>
+        <v>2.3865780000000001</v>
       </c>
       <c r="AH31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.17411899999999925</v>
+        <v>3.0041689999999992</v>
       </c>
       <c r="AI31">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2835819999999991</v>
+        <v>0.89470599999999934</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.2">
@@ -7786,139 +7802,139 @@
       </c>
       <c r="B32">
         <f t="shared" ref="B32:AI32" ca="1" si="2">ABS(B4-$AJ4)</f>
-        <v>6.6642569999999992</v>
+        <v>4.9171759999999995</v>
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="2"/>
-        <v>1.0992139999999999</v>
+        <v>0.64786699999999975</v>
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="2"/>
-        <v>6.6475000000000506E-2</v>
+        <v>1.8135560000000002</v>
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="2"/>
-        <v>1.0432360000000003</v>
+        <v>0.70384499999999939</v>
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="2"/>
-        <v>1.3276339999999998</v>
+        <v>0.4194469999999999</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0809620000000004</v>
+        <v>5.8280430000000001</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="2"/>
-        <v>5.6535030000000006</v>
+        <v>7.4005840000000003</v>
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="2"/>
-        <v>2.6030650000000009</v>
+        <v>4.3501460000000005</v>
       </c>
       <c r="J32">
         <f t="shared" ca="1" si="2"/>
-        <v>5.6535030000000006</v>
+        <v>7.4005840000000003</v>
       </c>
       <c r="K32">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5498180000000001</v>
+        <v>3.2968989999999998</v>
       </c>
       <c r="L32">
         <f t="shared" ca="1" si="2"/>
-        <v>1.3944419999999997</v>
+        <v>0.35263899999999992</v>
       </c>
       <c r="M32">
         <f t="shared" ca="1" si="2"/>
-        <v>0.77397399999999905</v>
+        <v>0.97310700000000061</v>
       </c>
       <c r="N32">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5163869999999999</v>
+        <v>0.23069399999999973</v>
       </c>
       <c r="O32">
         <f t="shared" ca="1" si="2"/>
-        <v>0.64559399999999911</v>
+        <v>1.1014870000000005</v>
       </c>
       <c r="P32">
         <f t="shared" ca="1" si="2"/>
-        <v>1.0119589999999992</v>
+        <v>0.7351220000000005</v>
       </c>
       <c r="Q32">
         <f t="shared" ca="1" si="2"/>
-        <v>3.9699410000000004</v>
+        <v>2.2228600000000007</v>
       </c>
       <c r="R32">
         <f t="shared" ca="1" si="2"/>
-        <v>4.9080130000000004</v>
+        <v>3.1609320000000007</v>
       </c>
       <c r="S32">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1235409999999995</v>
+        <v>1.3764599999999998</v>
       </c>
       <c r="T32">
         <f t="shared" ca="1" si="2"/>
-        <v>3.4892769999999995</v>
+        <v>1.7421959999999999</v>
       </c>
       <c r="U32">
         <f t="shared" ca="1" si="2"/>
-        <v>1.9149150000000006</v>
+        <v>0.16783400000000093</v>
       </c>
       <c r="V32">
         <f t="shared" si="2"/>
-        <v>11.984351</v>
+        <v>13.731432</v>
       </c>
       <c r="W32">
         <f t="shared" ca="1" si="2"/>
-        <v>11.984351</v>
+        <v>13.731432</v>
       </c>
       <c r="X32">
         <f t="shared" ca="1" si="2"/>
-        <v>11.984351</v>
+        <v>13.731432</v>
       </c>
       <c r="Y32">
         <f t="shared" ca="1" si="2"/>
-        <v>11.984351</v>
+        <v>13.731432</v>
       </c>
       <c r="Z32">
         <f t="shared" si="2"/>
-        <v>11.984351</v>
+        <v>13.731432</v>
       </c>
       <c r="AA32">
         <f t="shared" ca="1" si="2"/>
-        <v>3.8231950000000001</v>
+        <v>2.0761140000000005</v>
       </c>
       <c r="AB32">
         <f t="shared" ca="1" si="2"/>
-        <v>3.9511310000000002</v>
+        <v>2.2040500000000005</v>
       </c>
       <c r="AC32">
         <f t="shared" ca="1" si="2"/>
-        <v>3.7235279999999999</v>
+        <v>1.9764470000000003</v>
       </c>
       <c r="AD32">
         <f t="shared" ca="1" si="2"/>
-        <v>3.4257620000000006</v>
+        <v>1.678681000000001</v>
       </c>
       <c r="AE32">
         <f t="shared" ca="1" si="2"/>
-        <v>3.4613169999999993</v>
+        <v>1.7142359999999996</v>
       </c>
       <c r="AF32">
         <f t="shared" ca="1" si="2"/>
-        <v>3.8268249999999995</v>
+        <v>2.0797439999999998</v>
       </c>
       <c r="AG32">
         <f t="shared" ca="1" si="2"/>
-        <v>2.3560339999999993</v>
+        <v>0.60895299999999963</v>
       </c>
       <c r="AH32">
         <f t="shared" ca="1" si="2"/>
-        <v>2.6779499999999992</v>
+        <v>0.9308689999999995</v>
       </c>
       <c r="AI32">
         <f t="shared" ca="1" si="2"/>
-        <v>2.8581509999999994</v>
+        <v>1.1110699999999998</v>
       </c>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.2">
@@ -7927,139 +7943,139 @@
       </c>
       <c r="B33">
         <f t="shared" ref="B33:AI33" ca="1" si="3">ABS(B5-$AJ5)</f>
-        <v>0.79978599999999922</v>
+        <v>1.4657940000000007</v>
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="3"/>
-        <v>0.84921000000000113</v>
+        <v>0.18320199999999964</v>
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="3"/>
-        <v>0.99222399999999844</v>
+        <v>1.6582319999999999</v>
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="3"/>
-        <v>0.3699129999999986</v>
+        <v>1.0359210000000001</v>
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="3"/>
-        <v>0.11593799999999987</v>
+        <v>0.55007000000000161</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="3"/>
-        <v>0.21352599999999988</v>
+        <v>0.45248200000000161</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="3"/>
-        <v>2.8769749999999998</v>
+        <v>3.5429830000000013</v>
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="3"/>
-        <v>3.2819050000000001</v>
+        <v>3.9479130000000016</v>
       </c>
       <c r="J33">
         <f t="shared" ca="1" si="3"/>
-        <v>21.070156999999998</v>
+        <v>20.404148999999997</v>
       </c>
       <c r="K33">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9203799999999998</v>
+        <v>3.5863880000000012</v>
       </c>
       <c r="L33">
         <f t="shared" ca="1" si="3"/>
-        <v>0.23164100000000154</v>
+        <v>0.43436699999999995</v>
       </c>
       <c r="M33">
         <f t="shared" ca="1" si="3"/>
-        <v>0.97389699999999912</v>
+        <v>1.6399050000000006</v>
       </c>
       <c r="N33">
         <f t="shared" ca="1" si="3"/>
-        <v>0.40477399999999975</v>
+        <v>1.0707820000000012</v>
       </c>
       <c r="O33">
         <f t="shared" ca="1" si="3"/>
-        <v>0.76423899999999989</v>
+        <v>1.4302470000000014</v>
       </c>
       <c r="P33">
         <f t="shared" ca="1" si="3"/>
-        <v>4.829800000000084E-2</v>
+        <v>0.61771000000000065</v>
       </c>
       <c r="Q33">
         <f t="shared" ca="1" si="3"/>
-        <v>5.2984960000000001</v>
+        <v>4.6324879999999986</v>
       </c>
       <c r="R33">
         <f t="shared" ca="1" si="3"/>
-        <v>3.4862509999999993</v>
+        <v>2.8202429999999978</v>
       </c>
       <c r="S33">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9269540000000021</v>
+        <v>2.2609460000000006</v>
       </c>
       <c r="T33">
         <f t="shared" ca="1" si="3"/>
-        <v>4.8246560000000009</v>
+        <v>4.1586479999999995</v>
       </c>
       <c r="U33">
         <f t="shared" ca="1" si="3"/>
-        <v>2.7102180000000011</v>
+        <v>2.0442099999999996</v>
       </c>
       <c r="V33">
         <f t="shared" ca="1" si="3"/>
-        <v>20.302496000000001</v>
+        <v>19.636488</v>
       </c>
       <c r="W33">
         <f t="shared" ca="1" si="3"/>
-        <v>2.1653339999999996</v>
+        <v>2.8313420000000011</v>
       </c>
       <c r="X33">
         <f t="shared" ca="1" si="3"/>
-        <v>2.2367689999999989</v>
+        <v>2.9027770000000004</v>
       </c>
       <c r="Y33">
         <f t="shared" ca="1" si="3"/>
-        <v>4.2083099999999991</v>
+        <v>4.8743180000000006</v>
       </c>
       <c r="Z33">
         <f t="shared" ca="1" si="3"/>
-        <v>3.0663889999999991</v>
+        <v>3.7323970000000006</v>
       </c>
       <c r="AA33">
         <f t="shared" ca="1" si="3"/>
-        <v>1.0390290000000011</v>
+        <v>0.3730209999999996</v>
       </c>
       <c r="AB33">
         <f t="shared" ca="1" si="3"/>
-        <v>0.81804600000000072</v>
+        <v>0.15203799999999923</v>
       </c>
       <c r="AC33">
         <f t="shared" ca="1" si="3"/>
-        <v>1.7995760000000001</v>
+        <v>1.1335679999999986</v>
       </c>
       <c r="AD33">
         <f t="shared" ca="1" si="3"/>
-        <v>2.3964860000000012</v>
+        <v>1.7304779999999997</v>
       </c>
       <c r="AE33">
         <f t="shared" ca="1" si="3"/>
-        <v>0.70919500000000113</v>
+        <v>4.3186999999999642E-2</v>
       </c>
       <c r="AF33">
         <f t="shared" ca="1" si="3"/>
-        <v>2.4883820000000014</v>
+        <v>1.8223739999999999</v>
       </c>
       <c r="AG33">
         <f t="shared" ca="1" si="3"/>
-        <v>2.1018730000000012</v>
+        <v>1.4358649999999997</v>
       </c>
       <c r="AH33">
         <f t="shared" ca="1" si="3"/>
-        <v>0.28706500000000013</v>
+        <v>0.37894300000000136</v>
       </c>
       <c r="AI33">
         <f t="shared" ca="1" si="3"/>
-        <v>1.8021979999999989</v>
+        <v>2.4682060000000003</v>
       </c>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.2">
@@ -8068,91 +8084,91 @@
       </c>
       <c r="B34">
         <f t="shared" ref="B34:AI34" ca="1" si="4">ABS(B6-$AJ6)</f>
-        <v>2.160088</v>
+        <v>1.4705439999999985</v>
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="4"/>
-        <v>2.764069000000001</v>
+        <v>2.0745249999999995</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="4"/>
-        <v>1.9685550000000003</v>
+        <v>1.2790109999999988</v>
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="4"/>
-        <v>2.028378</v>
+        <v>1.3388339999999985</v>
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="4"/>
-        <v>2.1852499999999999</v>
+        <v>1.4957059999999984</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="4"/>
-        <v>6.1322889999999992</v>
+        <v>6.8218330000000007</v>
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="4"/>
-        <v>1.809177</v>
+        <v>1.1196329999999985</v>
       </c>
       <c r="I34">
         <f t="shared" ca="1" si="4"/>
-        <v>6.1322889999999992</v>
+        <v>6.8218330000000007</v>
       </c>
       <c r="J34">
         <f t="shared" ca="1" si="4"/>
-        <v>1.809177</v>
+        <v>1.1196329999999985</v>
       </c>
       <c r="K34">
         <f t="shared" ca="1" si="4"/>
-        <v>6.1322889999999992</v>
+        <v>6.8218330000000007</v>
       </c>
       <c r="L34">
         <f t="shared" ca="1" si="4"/>
-        <v>1.933605</v>
+        <v>1.2440609999999985</v>
       </c>
       <c r="M34">
         <f t="shared" ca="1" si="4"/>
-        <v>2.4246100000000013</v>
+        <v>1.7350659999999998</v>
       </c>
       <c r="N34">
         <f t="shared" ca="1" si="4"/>
-        <v>1.9226470000000013</v>
+        <v>1.2331029999999998</v>
       </c>
       <c r="O34">
         <f t="shared" ca="1" si="4"/>
-        <v>1.4102080000000008</v>
+        <v>0.72066399999999931</v>
       </c>
       <c r="P34">
         <f t="shared" ca="1" si="4"/>
-        <v>2.9437750000000005</v>
+        <v>2.254230999999999</v>
       </c>
       <c r="Q34">
         <f t="shared" ca="1" si="4"/>
-        <v>1.8001710000000006</v>
+        <v>1.1106269999999991</v>
       </c>
       <c r="R34">
         <f t="shared" ca="1" si="4"/>
-        <v>2.1738510000000009</v>
+        <v>1.4843069999999994</v>
       </c>
       <c r="S34">
         <f t="shared" ca="1" si="4"/>
-        <v>0.27989499999999978</v>
+        <v>0.40964900000000171</v>
       </c>
       <c r="T34">
         <f t="shared" ca="1" si="4"/>
-        <v>2.7566260000000007</v>
+        <v>2.0670819999999992</v>
       </c>
       <c r="U34">
         <f t="shared" ca="1" si="4"/>
-        <v>2.9744260000000011</v>
+        <v>2.2848819999999996</v>
       </c>
       <c r="V34">
         <f t="shared" ca="1" si="4"/>
-        <v>11.833567</v>
+        <v>11.144022999999999</v>
       </c>
       <c r="W34">
         <f t="shared" ca="1" si="4"/>
-        <v>8.7012310000000017</v>
+        <v>8.0116870000000002</v>
       </c>
       <c r="X34" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -8164,43 +8180,43 @@
       </c>
       <c r="Z34">
         <f t="shared" ca="1" si="4"/>
-        <v>6.4955580000000008</v>
+        <v>5.8060139999999993</v>
       </c>
       <c r="AA34">
         <f t="shared" ca="1" si="4"/>
-        <v>0.42803900000000006</v>
+        <v>0.26150500000000143</v>
       </c>
       <c r="AB34">
         <f t="shared" ca="1" si="4"/>
-        <v>1.067146000000001</v>
+        <v>0.37760199999999955</v>
       </c>
       <c r="AC34">
         <f t="shared" ca="1" si="4"/>
-        <v>0.41382000000000119</v>
+        <v>0.2757240000000003</v>
       </c>
       <c r="AD34">
         <f t="shared" ca="1" si="4"/>
-        <v>0.77327700000000021</v>
+        <v>8.3732999999998725E-2</v>
       </c>
       <c r="AE34">
         <f t="shared" ca="1" si="4"/>
-        <v>0.61730900000000055</v>
+        <v>7.2235000000000937E-2</v>
       </c>
       <c r="AF34">
         <f t="shared" ca="1" si="4"/>
-        <v>0.86339199999999927</v>
+        <v>1.5529360000000008</v>
       </c>
       <c r="AG34">
         <f t="shared" ca="1" si="4"/>
-        <v>0.33131000000000022</v>
+        <v>0.35823400000000127</v>
       </c>
       <c r="AH34">
         <f t="shared" ca="1" si="4"/>
-        <v>0.47000300000000017</v>
+        <v>0.21954100000000132</v>
       </c>
       <c r="AI34">
         <f t="shared" ca="1" si="4"/>
-        <v>0.1620980000000003</v>
+        <v>0.52744600000000119</v>
       </c>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.2">
@@ -8209,139 +8225,139 @@
       </c>
       <c r="B35">
         <f t="shared" ref="B35:AI35" ca="1" si="5">ABS(B7-$AJ7)</f>
-        <v>0.96476899999999866</v>
+        <v>0.12436499999999917</v>
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="5"/>
-        <v>1.55307</v>
+        <v>0.71266600000000047</v>
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="5"/>
-        <v>1.6050449999999987</v>
+        <v>0.76464099999999924</v>
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="5"/>
-        <v>1.0280759999999987</v>
+        <v>0.18767199999999917</v>
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="5"/>
-        <v>0.95792999999999928</v>
+        <v>0.1175259999999998</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="5"/>
-        <v>3.5202720000000003</v>
+        <v>2.6798680000000008</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="5"/>
-        <v>3.1084870000000002</v>
+        <v>2.2680830000000007</v>
       </c>
       <c r="I35">
         <f t="shared" si="5"/>
-        <v>12.808600999999999</v>
+        <v>11.968197</v>
       </c>
       <c r="J35">
         <f t="shared" si="5"/>
-        <v>12.808600999999999</v>
+        <v>11.968197</v>
       </c>
       <c r="K35">
         <f t="shared" si="5"/>
-        <v>12.808600999999999</v>
+        <v>11.968197</v>
       </c>
       <c r="L35">
         <f t="shared" ca="1" si="5"/>
-        <v>0.88934099999999994</v>
+        <v>4.8937000000000452E-2</v>
       </c>
       <c r="M35">
         <f t="shared" ca="1" si="5"/>
-        <v>0.75625699999999973</v>
+        <v>8.414699999999975E-2</v>
       </c>
       <c r="N35">
         <f t="shared" ca="1" si="5"/>
-        <v>0.96355299999999922</v>
+        <v>0.12314899999999973</v>
       </c>
       <c r="O35">
         <f t="shared" ca="1" si="5"/>
-        <v>0.66946599999999989</v>
+        <v>0.17093799999999959</v>
       </c>
       <c r="P35">
         <f t="shared" ca="1" si="5"/>
-        <v>0.50982400000000005</v>
+        <v>0.33057999999999943</v>
       </c>
       <c r="Q35">
         <f t="shared" ca="1" si="5"/>
-        <v>0.85067500000000074</v>
+        <v>1.6910790000000002</v>
       </c>
       <c r="R35">
         <f t="shared" ca="1" si="5"/>
-        <v>1.5675999999999135E-2</v>
+        <v>0.82472800000000035</v>
       </c>
       <c r="S35">
         <f t="shared" ca="1" si="5"/>
-        <v>0.84937799999999974</v>
+        <v>1.6897819999999992</v>
       </c>
       <c r="T35">
         <f t="shared" ca="1" si="5"/>
-        <v>1.0122689999999999</v>
+        <v>1.8526729999999993</v>
       </c>
       <c r="U35">
         <f t="shared" ca="1" si="5"/>
-        <v>1.7957910000000012</v>
+        <v>2.6361950000000007</v>
       </c>
       <c r="V35">
         <f t="shared" ca="1" si="5"/>
-        <v>5.9129730000000009</v>
+        <v>6.7533770000000004</v>
       </c>
       <c r="W35">
         <f t="shared" ca="1" si="5"/>
-        <v>4.8506529999999994</v>
+        <v>4.010249</v>
       </c>
       <c r="X35">
         <f t="shared" ca="1" si="5"/>
-        <v>3.7102379999999986</v>
+        <v>2.8698339999999991</v>
       </c>
       <c r="Y35">
         <f t="shared" ca="1" si="5"/>
-        <v>5.5740489999999996</v>
+        <v>4.7336450000000001</v>
       </c>
       <c r="Z35">
         <f t="shared" ca="1" si="5"/>
-        <v>3.4492209999999996</v>
+        <v>2.6088170000000002</v>
       </c>
       <c r="AA35">
         <f t="shared" ca="1" si="5"/>
-        <v>0.22429699999999997</v>
+        <v>0.61610699999999952</v>
       </c>
       <c r="AB35">
         <f t="shared" ca="1" si="5"/>
-        <v>0.39864299999999986</v>
+        <v>0.44176099999999963</v>
       </c>
       <c r="AC35">
         <f t="shared" ca="1" si="5"/>
-        <v>0.27185400000000115</v>
+        <v>1.1122580000000006</v>
       </c>
       <c r="AD35">
         <f t="shared" ca="1" si="5"/>
-        <v>0.63258999999999865</v>
+        <v>0.20781400000000083</v>
       </c>
       <c r="AE35">
         <f t="shared" ca="1" si="5"/>
-        <v>0.53670299999999926</v>
+        <v>0.30370100000000022</v>
       </c>
       <c r="AF35">
         <f t="shared" ca="1" si="5"/>
-        <v>0.68003199999999886</v>
+        <v>0.16037200000000063</v>
       </c>
       <c r="AG35">
         <f t="shared" ca="1" si="5"/>
-        <v>4.9787000000000248E-2</v>
+        <v>0.79061699999999924</v>
       </c>
       <c r="AH35">
         <f t="shared" ca="1" si="5"/>
-        <v>0.73752300000000126</v>
+        <v>1.5779270000000007</v>
       </c>
       <c r="AI35">
         <f t="shared" ca="1" si="5"/>
-        <v>1.3177880000000002</v>
+        <v>0.4773840000000007</v>
       </c>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.2">
@@ -8350,87 +8366,87 @@
       </c>
       <c r="B36">
         <f t="shared" ref="B36:AI36" ca="1" si="6">ABS(B8-$AJ8)</f>
-        <v>2.6606860000000001</v>
+        <v>1.733353000000001</v>
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="6"/>
-        <v>2.7225470000000005</v>
+        <v>1.7952140000000014</v>
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="6"/>
-        <v>3.3092639999999989</v>
+        <v>2.3819309999999998</v>
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="6"/>
-        <v>2.6238150000000005</v>
+        <v>1.6964820000000014</v>
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="6"/>
-        <v>2.6926259999999989</v>
+        <v>1.7652929999999998</v>
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="6"/>
-        <v>3.4916260000000001</v>
+        <v>2.564293000000001</v>
       </c>
       <c r="H36">
         <f t="shared" si="6"/>
-        <v>8.9597800000000003</v>
+        <v>9.8871129999999994</v>
       </c>
       <c r="I36">
         <f t="shared" si="6"/>
-        <v>8.9597800000000003</v>
+        <v>9.8871129999999994</v>
       </c>
       <c r="J36">
         <f t="shared" si="6"/>
-        <v>8.9597800000000003</v>
+        <v>9.8871129999999994</v>
       </c>
       <c r="K36">
         <f t="shared" si="6"/>
-        <v>8.9597800000000003</v>
+        <v>9.8871129999999994</v>
       </c>
       <c r="L36">
         <f t="shared" ca="1" si="6"/>
-        <v>2.4511389999999995</v>
+        <v>1.5238060000000004</v>
       </c>
       <c r="M36">
         <f t="shared" ca="1" si="6"/>
-        <v>3.3043759999999995</v>
+        <v>2.3770430000000005</v>
       </c>
       <c r="N36">
         <f t="shared" ca="1" si="6"/>
-        <v>3.3091039999999996</v>
+        <v>2.3817710000000005</v>
       </c>
       <c r="O36">
         <f t="shared" ca="1" si="6"/>
-        <v>3.1238039999999998</v>
+        <v>2.1964710000000007</v>
       </c>
       <c r="P36">
         <f t="shared" ca="1" si="6"/>
-        <v>2.7104509999999991</v>
+        <v>1.783118</v>
       </c>
       <c r="Q36">
         <f t="shared" ca="1" si="6"/>
-        <v>5.9493220000000004</v>
+        <v>5.0219890000000014</v>
       </c>
       <c r="R36">
         <f t="shared" ca="1" si="6"/>
-        <v>2.2586309999999994</v>
+        <v>1.3312980000000003</v>
       </c>
       <c r="S36">
         <f t="shared" ca="1" si="6"/>
-        <v>3.0296599999999998</v>
+        <v>2.1023270000000007</v>
       </c>
       <c r="T36">
         <f t="shared" ca="1" si="6"/>
-        <v>2.456925</v>
+        <v>1.529592000000001</v>
       </c>
       <c r="U36">
         <f t="shared" ca="1" si="6"/>
-        <v>2.3427679999999995</v>
+        <v>1.4154350000000004</v>
       </c>
       <c r="V36">
         <f t="shared" ca="1" si="6"/>
-        <v>7.2432530000000011</v>
+        <v>6.315920000000002</v>
       </c>
       <c r="W36" t="e">
         <f t="shared" ca="1" si="6"/>
@@ -8442,43 +8458,43 @@
       </c>
       <c r="Y36">
         <f t="shared" ca="1" si="6"/>
-        <v>23.134388000000001</v>
+        <v>22.207055000000004</v>
       </c>
       <c r="AA36">
         <f t="shared" ca="1" si="6"/>
-        <v>2.7097470000000001</v>
+        <v>1.7824140000000011</v>
       </c>
       <c r="AB36">
         <f t="shared" ca="1" si="6"/>
-        <v>1.3827929999999995</v>
+        <v>0.45546000000000042</v>
       </c>
       <c r="AC36">
         <f t="shared" ca="1" si="6"/>
-        <v>2.522473999999999</v>
+        <v>1.5951409999999999</v>
       </c>
       <c r="AD36">
         <f t="shared" ca="1" si="6"/>
-        <v>1.8169900000000005</v>
+        <v>0.88965700000000147</v>
       </c>
       <c r="AE36">
         <f t="shared" ca="1" si="6"/>
-        <v>2.3898849999999996</v>
+        <v>1.4625520000000005</v>
       </c>
       <c r="AF36">
         <f t="shared" ca="1" si="6"/>
-        <v>1.2281279999999999</v>
+        <v>0.30079500000000081</v>
       </c>
       <c r="AG36">
         <f t="shared" ca="1" si="6"/>
-        <v>1.503563999999999</v>
+        <v>0.57623099999999994</v>
       </c>
       <c r="AH36">
         <f t="shared" ca="1" si="6"/>
-        <v>1.3482029999999998</v>
+        <v>0.42087000000000074</v>
       </c>
       <c r="AI36">
         <f t="shared" ca="1" si="6"/>
-        <v>1.4034219999999991</v>
+        <v>0.47608899999999998</v>
       </c>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.2">
@@ -8487,139 +8503,139 @@
       </c>
       <c r="B37">
         <f t="shared" ref="B37:AI37" ca="1" si="7">ABS(B9-$AJ9)</f>
-        <v>2.1941640000000007</v>
+        <v>2.4906459999999999</v>
       </c>
       <c r="C37">
         <f t="shared" ca="1" si="7"/>
-        <v>1.8837109999999999</v>
+        <v>2.1801929999999992</v>
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="7"/>
-        <v>2.5739809999999999</v>
+        <v>2.8704629999999991</v>
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="7"/>
-        <v>1.9174749999999996</v>
+        <v>2.2139569999999988</v>
       </c>
       <c r="F37">
         <f t="shared" ca="1" si="7"/>
-        <v>1.9286410000000007</v>
+        <v>2.225123</v>
       </c>
       <c r="G37">
         <f t="shared" si="7"/>
-        <v>9.59863</v>
+        <v>9.3021480000000007</v>
       </c>
       <c r="H37">
         <f t="shared" si="7"/>
-        <v>9.59863</v>
+        <v>9.3021480000000007</v>
       </c>
       <c r="I37">
         <f t="shared" ca="1" si="7"/>
-        <v>27.917969999999997</v>
+        <v>28.214451999999994</v>
       </c>
       <c r="J37">
         <f t="shared" si="7"/>
-        <v>9.59863</v>
+        <v>9.3021480000000007</v>
       </c>
       <c r="K37">
         <f t="shared" si="7"/>
-        <v>9.59863</v>
+        <v>9.3021480000000007</v>
       </c>
       <c r="L37">
         <f t="shared" ca="1" si="7"/>
-        <v>0.92005999999999943</v>
+        <v>1.2165419999999987</v>
       </c>
       <c r="M37">
         <f t="shared" ca="1" si="7"/>
-        <v>1.7071679999999994</v>
+        <v>2.0036499999999986</v>
       </c>
       <c r="N37">
         <f t="shared" ca="1" si="7"/>
-        <v>1.0115630000000007</v>
+        <v>1.3080449999999999</v>
       </c>
       <c r="O37">
         <f t="shared" ca="1" si="7"/>
-        <v>1.4971890000000005</v>
+        <v>1.7936709999999998</v>
       </c>
       <c r="P37">
         <f t="shared" ca="1" si="7"/>
-        <v>2.0101800000000001</v>
+        <v>2.3066619999999993</v>
       </c>
       <c r="Q37">
         <f t="shared" ca="1" si="7"/>
-        <v>2.0690760000000008</v>
+        <v>2.365558</v>
       </c>
       <c r="R37">
         <f t="shared" ca="1" si="7"/>
-        <v>2.5530209999999993</v>
+        <v>2.8495029999999986</v>
       </c>
       <c r="S37">
         <f t="shared" ca="1" si="7"/>
-        <v>2.6863829999999993</v>
+        <v>2.9828649999999985</v>
       </c>
       <c r="T37">
         <f t="shared" ca="1" si="7"/>
-        <v>1.8959530000000004</v>
+        <v>2.1924349999999997</v>
       </c>
       <c r="U37">
         <f t="shared" ca="1" si="7"/>
-        <v>1.3611050000000002</v>
+        <v>1.6575869999999995</v>
       </c>
       <c r="V37">
         <f t="shared" ca="1" si="7"/>
-        <v>0.27991899999999958</v>
+        <v>0.57640099999999883</v>
       </c>
       <c r="W37">
         <f t="shared" ca="1" si="7"/>
-        <v>0.12451599999999985</v>
+        <v>0.1719659999999994</v>
       </c>
       <c r="X37">
         <f t="shared" ca="1" si="7"/>
-        <v>4.0629779999999993</v>
+        <v>4.3594599999999986</v>
       </c>
       <c r="Y37">
         <f t="shared" ca="1" si="7"/>
-        <v>47.796117000000002</v>
+        <v>48.092599</v>
       </c>
       <c r="Z37">
         <f t="shared" ca="1" si="7"/>
-        <v>3.925243</v>
+        <v>4.2217249999999993</v>
       </c>
       <c r="AA37">
         <f t="shared" ca="1" si="7"/>
-        <v>0.46267800000000037</v>
+        <v>0.75915999999999961</v>
       </c>
       <c r="AB37">
         <f t="shared" ca="1" si="7"/>
-        <v>1.5312049999999999</v>
+        <v>1.8276869999999992</v>
       </c>
       <c r="AC37">
         <f t="shared" ca="1" si="7"/>
-        <v>0.7353310000000004</v>
+        <v>1.0318129999999996</v>
       </c>
       <c r="AD37">
         <f t="shared" ca="1" si="7"/>
-        <v>0.26245399999999997</v>
+        <v>0.55893599999999921</v>
       </c>
       <c r="AE37">
         <f t="shared" ca="1" si="7"/>
-        <v>0.77957199999999993</v>
+        <v>1.0760539999999992</v>
       </c>
       <c r="AF37">
         <f t="shared" ca="1" si="7"/>
-        <v>0.32776499999999942</v>
+        <v>0.62424699999999866</v>
       </c>
       <c r="AG37">
         <f t="shared" ca="1" si="7"/>
-        <v>0.1813059999999993</v>
+        <v>0.47778799999999855</v>
       </c>
       <c r="AH37">
         <f t="shared" ca="1" si="7"/>
-        <v>9.7537000000000873E-2</v>
+        <v>0.39401900000000012</v>
       </c>
       <c r="AI37">
         <f t="shared" ca="1" si="7"/>
-        <v>0.47882899999999928</v>
+        <v>0.77531099999999853</v>
       </c>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.2">
@@ -8628,139 +8644,139 @@
       </c>
       <c r="B38">
         <f t="shared" ref="B38:AI38" ca="1" si="8">ABS(B10-$AJ10)</f>
-        <v>3.6283449999999995</v>
+        <v>3.8806700000000003</v>
       </c>
       <c r="C38">
         <f t="shared" ca="1" si="8"/>
-        <v>0.7913610000000002</v>
+        <v>1.043686000000001</v>
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="8"/>
-        <v>1.7234379999999998</v>
+        <v>1.9757630000000006</v>
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="8"/>
-        <v>1.5264749999999996</v>
+        <v>1.7788000000000004</v>
       </c>
       <c r="F38">
         <f t="shared" ca="1" si="8"/>
-        <v>3.7661519999999999</v>
+        <v>4.0184770000000007</v>
       </c>
       <c r="G38">
         <f t="shared" ca="1" si="8"/>
-        <v>0.71714300000000009</v>
+        <v>0.96946800000000088</v>
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="8"/>
-        <v>0.71714300000000009</v>
+        <v>0.96946800000000088</v>
       </c>
       <c r="I38">
         <f t="shared" ca="1" si="8"/>
-        <v>3.287058</v>
+        <v>3.0347329999999992</v>
       </c>
       <c r="J38">
         <f t="shared" ca="1" si="8"/>
-        <v>0.71714300000000009</v>
+        <v>0.96946800000000088</v>
       </c>
       <c r="K38">
         <f t="shared" ca="1" si="8"/>
-        <v>1.0755379999999999</v>
+        <v>0.82321299999999908</v>
       </c>
       <c r="L38">
         <f t="shared" ca="1" si="8"/>
-        <v>2.9740760000000002</v>
+        <v>3.226401000000001</v>
       </c>
       <c r="M38">
         <f t="shared" ca="1" si="8"/>
-        <v>2.4268169999999998</v>
+        <v>2.6791420000000006</v>
       </c>
       <c r="N38">
         <f t="shared" ca="1" si="8"/>
-        <v>1.7656569999999991</v>
+        <v>2.0179819999999999</v>
       </c>
       <c r="O38">
         <f t="shared" ca="1" si="8"/>
-        <v>1.8811389999999992</v>
+        <v>2.133464</v>
       </c>
       <c r="P38">
         <f t="shared" ca="1" si="8"/>
-        <v>2.5319590000000005</v>
+        <v>2.7842840000000013</v>
       </c>
       <c r="Q38">
         <f t="shared" ca="1" si="8"/>
-        <v>2.6846599999999992</v>
+        <v>2.936985</v>
       </c>
       <c r="R38">
         <f t="shared" ca="1" si="8"/>
-        <v>4.1353880000000007</v>
+        <v>4.3877130000000015</v>
       </c>
       <c r="S38">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8915950000000006</v>
+        <v>3.1439200000000014</v>
       </c>
       <c r="T38">
         <f t="shared" ca="1" si="8"/>
-        <v>5.3440739999999991</v>
+        <v>5.5963989999999999</v>
       </c>
       <c r="U38">
         <f t="shared" ca="1" si="8"/>
-        <v>5.6462819999999994</v>
+        <v>5.8986070000000002</v>
       </c>
       <c r="V38">
         <f t="shared" ca="1" si="8"/>
-        <v>4.7109729999999992</v>
+        <v>4.963298</v>
       </c>
       <c r="W38">
         <f t="shared" ca="1" si="8"/>
-        <v>0.15740899999999947</v>
+        <v>0.40973400000000026</v>
       </c>
       <c r="X38">
         <f t="shared" ca="1" si="8"/>
-        <v>5.2669200000000007</v>
+        <v>5.5192450000000015</v>
       </c>
       <c r="Y38">
         <f t="shared" ca="1" si="8"/>
-        <v>0.10854999999999926</v>
+        <v>0.36087500000000006</v>
       </c>
       <c r="Z38">
         <f t="shared" ca="1" si="8"/>
-        <v>5.0204409999999999</v>
+        <v>5.2727660000000007</v>
       </c>
       <c r="AA38">
         <f t="shared" ca="1" si="8"/>
-        <v>1.8575119999999998</v>
+        <v>2.1098370000000006</v>
       </c>
       <c r="AB38">
         <f t="shared" ca="1" si="8"/>
-        <v>2.1318249999999992</v>
+        <v>2.38415</v>
       </c>
       <c r="AC38">
         <f t="shared" ca="1" si="8"/>
-        <v>1.644088</v>
+        <v>1.8964130000000008</v>
       </c>
       <c r="AD38">
         <f t="shared" ca="1" si="8"/>
-        <v>1.1444600000000005</v>
+        <v>1.3967850000000013</v>
       </c>
       <c r="AE38">
         <f t="shared" ca="1" si="8"/>
-        <v>2.0805810000000005</v>
+        <v>2.3329060000000013</v>
       </c>
       <c r="AF38">
         <f t="shared" ca="1" si="8"/>
-        <v>1.5506829999999994</v>
+        <v>1.8030080000000002</v>
       </c>
       <c r="AG38">
         <f t="shared" ca="1" si="8"/>
-        <v>1.0655699999999992</v>
+        <v>1.317895</v>
       </c>
       <c r="AH38">
         <f t="shared" ca="1" si="8"/>
-        <v>0.53445299999999918</v>
+        <v>0.78677799999999998</v>
       </c>
       <c r="AI38">
         <f t="shared" ca="1" si="8"/>
-        <v>0.56625299999999967</v>
+        <v>0.81857800000000047</v>
       </c>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.2">
@@ -8769,139 +8785,139 @@
       </c>
       <c r="B39">
         <f t="shared" ref="B39:AI39" ca="1" si="9">ABS(B11-$AJ11)</f>
-        <v>1.192202</v>
+        <v>1.8096990000000002</v>
       </c>
       <c r="C39">
         <f t="shared" ca="1" si="9"/>
-        <v>1.2425189999999997</v>
+        <v>1.8600159999999999</v>
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="9"/>
-        <v>2.3007549999999988</v>
+        <v>2.918251999999999</v>
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="9"/>
-        <v>2.3541329999999991</v>
+        <v>2.9716299999999993</v>
       </c>
       <c r="F39">
         <f t="shared" ca="1" si="9"/>
-        <v>2.1248249999999995</v>
+        <v>2.7423219999999997</v>
       </c>
       <c r="G39">
         <f t="shared" ca="1" si="9"/>
-        <v>6.6232099999999985</v>
+        <v>7.2407069999999987</v>
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="9"/>
-        <v>6.6232099999999985</v>
+        <v>7.2407069999999987</v>
       </c>
       <c r="I39">
         <f t="shared" ca="1" si="9"/>
-        <v>5.1778999999999993</v>
+        <v>5.7953969999999995</v>
       </c>
       <c r="J39">
         <f t="shared" ca="1" si="9"/>
-        <v>18.874586999999998</v>
+        <v>19.492083999999998</v>
       </c>
       <c r="K39">
         <f t="shared" ca="1" si="9"/>
-        <v>10009.516170000001</v>
+        <v>10008.898673</v>
       </c>
       <c r="L39">
         <f t="shared" ca="1" si="9"/>
-        <v>0.88382999999999967</v>
+        <v>1.5013269999999999</v>
       </c>
       <c r="M39">
         <f t="shared" ca="1" si="9"/>
-        <v>1.5409039999999994</v>
+        <v>2.1584009999999996</v>
       </c>
       <c r="N39">
         <f t="shared" ca="1" si="9"/>
-        <v>1.0985239999999994</v>
+        <v>1.7160209999999996</v>
       </c>
       <c r="O39">
         <f t="shared" ca="1" si="9"/>
-        <v>1.2425189999999997</v>
+        <v>1.8600159999999999</v>
       </c>
       <c r="P39">
         <f t="shared" ca="1" si="9"/>
-        <v>1.6786370000000002</v>
+        <v>2.2961340000000003</v>
       </c>
       <c r="Q39">
         <f t="shared" ca="1" si="9"/>
-        <v>3.9373689999999986</v>
+        <v>4.5548659999999987</v>
       </c>
       <c r="R39">
         <f t="shared" ca="1" si="9"/>
-        <v>1.8422149999999995</v>
+        <v>2.4597119999999997</v>
       </c>
       <c r="S39">
         <f t="shared" ca="1" si="9"/>
-        <v>2.1360890000000001</v>
+        <v>2.7535860000000003</v>
       </c>
       <c r="T39">
         <f t="shared" ca="1" si="9"/>
-        <v>0.60950300000000013</v>
+        <v>1.2270000000000003</v>
       </c>
       <c r="U39">
         <f t="shared" ca="1" si="9"/>
-        <v>1.7210219999999996</v>
+        <v>2.3385189999999998</v>
       </c>
       <c r="V39">
         <f t="shared" ca="1" si="9"/>
-        <v>1.6999040000000001</v>
+        <v>2.3174010000000003</v>
       </c>
       <c r="W39">
         <f t="shared" ca="1" si="9"/>
-        <v>3.7593029999999992</v>
+        <v>4.3767999999999994</v>
       </c>
       <c r="X39">
         <f t="shared" ca="1" si="9"/>
-        <v>1.989198</v>
+        <v>2.6066950000000002</v>
       </c>
       <c r="Y39">
         <f t="shared" ca="1" si="9"/>
-        <v>2.0511510000000008</v>
+        <v>1.4336540000000007</v>
       </c>
       <c r="Z39">
         <f t="shared" ca="1" si="9"/>
-        <v>0.74877100000000141</v>
+        <v>0.13127400000000122</v>
       </c>
       <c r="AA39">
         <f t="shared" ca="1" si="9"/>
-        <v>0.60432400000000008</v>
+        <v>1.2218210000000003</v>
       </c>
       <c r="AB39">
         <f t="shared" ca="1" si="9"/>
-        <v>1.2695179999999997</v>
+        <v>1.8870149999999999</v>
       </c>
       <c r="AC39">
         <f t="shared" ca="1" si="9"/>
-        <v>0.15625299999999953</v>
+        <v>0.77374999999999972</v>
       </c>
       <c r="AD39">
         <f t="shared" ca="1" si="9"/>
-        <v>0.86723499999999909</v>
+        <v>1.4847319999999993</v>
       </c>
       <c r="AE39">
         <f t="shared" ca="1" si="9"/>
-        <v>0.54859699999999911</v>
+        <v>1.1660939999999993</v>
       </c>
       <c r="AF39">
         <f t="shared" ca="1" si="9"/>
-        <v>0.42597100000000054</v>
+        <v>0.19152599999999964</v>
       </c>
       <c r="AG39">
         <f t="shared" ca="1" si="9"/>
-        <v>0.90246800000000071</v>
+        <v>0.28497100000000053</v>
       </c>
       <c r="AH39">
         <f t="shared" ca="1" si="9"/>
-        <v>0.7445320000000013</v>
+        <v>0.12703500000000112</v>
       </c>
       <c r="AI39">
         <f t="shared" ca="1" si="9"/>
-        <v>0.8651440000000008</v>
+        <v>0.24764700000000062</v>
       </c>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.2">
@@ -8910,139 +8926,139 @@
       </c>
       <c r="B40">
         <f t="shared" ref="B40:AI40" ca="1" si="10">ABS(B12-$AJ12)</f>
-        <v>2.0162040000000001</v>
+        <v>0.53267100000000056</v>
       </c>
       <c r="C40">
         <f t="shared" ca="1" si="10"/>
-        <v>1.7146810000000006</v>
+        <v>0.23114800000000102</v>
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="10"/>
-        <v>1.3277000000000001</v>
+        <v>0.15583299999999944</v>
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="10"/>
-        <v>1.755217</v>
+        <v>0.27168400000000048</v>
       </c>
       <c r="F40">
         <f t="shared" ca="1" si="10"/>
-        <v>1.3990000000000009</v>
+        <v>8.4532999999998637E-2</v>
       </c>
       <c r="G40">
         <f t="shared" ca="1" si="10"/>
-        <v>20.952069000000002</v>
+        <v>22.435601999999999</v>
       </c>
       <c r="H40">
         <f t="shared" si="10"/>
-        <v>9.5465809999999998</v>
+        <v>11.030113999999999</v>
       </c>
       <c r="I40">
         <f t="shared" si="10"/>
-        <v>9.5465809999999998</v>
+        <v>11.030113999999999</v>
       </c>
       <c r="J40">
         <f t="shared" si="10"/>
-        <v>9.5465809999999998</v>
+        <v>11.030113999999999</v>
       </c>
       <c r="K40">
         <f t="shared" ca="1" si="10"/>
-        <v>19.362991999999998</v>
+        <v>20.846525</v>
       </c>
       <c r="L40">
         <f t="shared" ca="1" si="10"/>
-        <v>0.60169600000000045</v>
+        <v>0.88183699999999909</v>
       </c>
       <c r="M40">
         <f t="shared" ca="1" si="10"/>
-        <v>0.67927599999999977</v>
+        <v>0.80425699999999978</v>
       </c>
       <c r="N40">
         <f t="shared" ca="1" si="10"/>
-        <v>0.44524400000000064</v>
+        <v>1.0382889999999989</v>
       </c>
       <c r="O40">
         <f t="shared" ca="1" si="10"/>
-        <v>0.73212999999999973</v>
+        <v>0.75140299999999982</v>
       </c>
       <c r="P40">
         <f t="shared" ca="1" si="10"/>
-        <v>0.13148100000000085</v>
+        <v>1.3520519999999987</v>
       </c>
       <c r="Q40">
         <f t="shared" ca="1" si="10"/>
-        <v>1.9787920000000003</v>
+        <v>0.49525900000000078</v>
       </c>
       <c r="R40">
         <f t="shared" ca="1" si="10"/>
-        <v>0.27594299999999983</v>
+        <v>1.7594759999999994</v>
       </c>
       <c r="S40">
         <f t="shared" ca="1" si="10"/>
-        <v>0.4172349999999998</v>
+        <v>1.0662979999999997</v>
       </c>
       <c r="T40">
         <f t="shared" ca="1" si="10"/>
-        <v>0.31138400000000033</v>
+        <v>1.7949169999999999</v>
       </c>
       <c r="U40">
         <f t="shared" ca="1" si="10"/>
-        <v>0.31306999999999974</v>
+        <v>1.1704629999999998</v>
       </c>
       <c r="V40">
         <f t="shared" ca="1" si="10"/>
-        <v>3.8954240000000002</v>
+        <v>2.4118910000000007</v>
       </c>
       <c r="W40">
         <f t="shared" ca="1" si="10"/>
-        <v>5.9875640000000008</v>
+        <v>4.5040310000000012</v>
       </c>
       <c r="X40">
         <f t="shared" ca="1" si="10"/>
-        <v>3.8954240000000002</v>
+        <v>2.4118910000000007</v>
       </c>
       <c r="Y40">
         <f t="shared" ca="1" si="10"/>
-        <v>1.7753379999999996</v>
+        <v>0.29180500000000009</v>
       </c>
       <c r="Z40">
         <f t="shared" ca="1" si="10"/>
-        <v>8.7761859999999992</v>
+        <v>7.2926529999999996</v>
       </c>
       <c r="AA40">
         <f t="shared" ca="1" si="10"/>
-        <v>0.30636300000000105</v>
+        <v>1.1771699999999985</v>
       </c>
       <c r="AB40">
         <f t="shared" ca="1" si="10"/>
-        <v>0.22578200000000059</v>
+        <v>1.257750999999999</v>
       </c>
       <c r="AC40">
         <f t="shared" ca="1" si="10"/>
-        <v>6.3264999999999461E-2</v>
+        <v>1.4202680000000001</v>
       </c>
       <c r="AD40">
         <f t="shared" ca="1" si="10"/>
-        <v>0.38846700000000034</v>
+        <v>1.8719999999999999</v>
       </c>
       <c r="AE40">
         <f t="shared" ca="1" si="10"/>
-        <v>8.3622999999999337E-2</v>
+        <v>1.5671559999999989</v>
       </c>
       <c r="AF40">
         <f t="shared" ca="1" si="10"/>
-        <v>0.60010199999999969</v>
+        <v>2.0836349999999992</v>
       </c>
       <c r="AG40">
         <f t="shared" ca="1" si="10"/>
-        <v>8.6307999999998941E-2</v>
+        <v>1.5698409999999985</v>
       </c>
       <c r="AH40">
         <f t="shared" ca="1" si="10"/>
-        <v>0.45969000000000015</v>
+        <v>1.9432229999999997</v>
       </c>
       <c r="AI40">
         <f t="shared" ca="1" si="10"/>
-        <v>0.70534600000000047</v>
+        <v>2.188879</v>
       </c>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.2">
@@ -9051,139 +9067,139 @@
       </c>
       <c r="B41">
         <f t="shared" ref="B41:AI41" ca="1" si="11">ABS(B13-$AJ13)</f>
-        <v>0.64841399999999894</v>
+        <v>0.78517899999999941</v>
       </c>
       <c r="C41">
         <f t="shared" ca="1" si="11"/>
-        <v>0.62061800000000034</v>
+        <v>0.48385299999999987</v>
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="11"/>
-        <v>0.1700430000000015</v>
+        <v>3.3278000000001029E-2</v>
       </c>
       <c r="E41">
         <f t="shared" ca="1" si="11"/>
-        <v>0.94093100000000085</v>
+        <v>0.80416600000000038</v>
       </c>
       <c r="F41">
         <f t="shared" ca="1" si="11"/>
-        <v>1.2542840000000002</v>
+        <v>1.1175189999999997</v>
       </c>
       <c r="G41">
         <f t="shared" si="11"/>
-        <v>8.3988029999999991</v>
+        <v>8.5355679999999996</v>
       </c>
       <c r="H41">
         <f t="shared" si="11"/>
-        <v>8.3988029999999991</v>
+        <v>8.5355679999999996</v>
       </c>
       <c r="I41">
         <f t="shared" ca="1" si="11"/>
-        <v>7.8693509999999991</v>
+        <v>8.0061159999999987</v>
       </c>
       <c r="J41">
         <f t="shared" si="11"/>
-        <v>8.3988029999999991</v>
+        <v>8.5355679999999996</v>
       </c>
       <c r="K41">
         <f t="shared" si="11"/>
-        <v>8.3988029999999991</v>
+        <v>8.5355679999999996</v>
       </c>
       <c r="L41">
         <f t="shared" ca="1" si="11"/>
-        <v>3.7044890000000006</v>
+        <v>3.5677240000000001</v>
       </c>
       <c r="M41">
         <f t="shared" ca="1" si="11"/>
-        <v>3.3228460000000002</v>
+        <v>3.1860809999999997</v>
       </c>
       <c r="N41">
         <f t="shared" ca="1" si="11"/>
-        <v>2.9306190000000001</v>
+        <v>2.7938539999999996</v>
       </c>
       <c r="O41">
         <f t="shared" ca="1" si="11"/>
-        <v>3.1087730000000011</v>
+        <v>2.9720080000000006</v>
       </c>
       <c r="P41">
         <f t="shared" ca="1" si="11"/>
-        <v>2.7420530000000003</v>
+        <v>2.6052879999999998</v>
       </c>
       <c r="Q41">
         <f t="shared" ca="1" si="11"/>
-        <v>2.6385190000000005</v>
+        <v>2.501754</v>
       </c>
       <c r="R41">
         <f t="shared" ca="1" si="11"/>
-        <v>2.4558650000000011</v>
+        <v>2.3191000000000006</v>
       </c>
       <c r="S41">
         <f t="shared" ca="1" si="11"/>
-        <v>3.0212640000000004</v>
+        <v>2.8844989999999999</v>
       </c>
       <c r="T41">
         <f t="shared" ca="1" si="11"/>
-        <v>2.3431270000000008</v>
+        <v>2.2063620000000004</v>
       </c>
       <c r="U41">
         <f t="shared" ca="1" si="11"/>
-        <v>3.2188180000000006</v>
+        <v>3.0820530000000002</v>
       </c>
       <c r="V41">
         <f t="shared" ca="1" si="11"/>
-        <v>11.887683000000001</v>
+        <v>11.750918</v>
       </c>
       <c r="W41">
         <f t="shared" ca="1" si="11"/>
-        <v>19.640844999999999</v>
+        <v>19.504080000000002</v>
       </c>
       <c r="X41">
         <f t="shared" ca="1" si="11"/>
-        <v>34.596285999999999</v>
+        <v>34.459521000000002</v>
       </c>
       <c r="Y41">
         <f t="shared" ca="1" si="11"/>
-        <v>0.7701829999999994</v>
+        <v>0.90694799999999987</v>
       </c>
       <c r="Z41">
         <f t="shared" ca="1" si="11"/>
-        <v>11.738256000000002</v>
+        <v>11.601491000000001</v>
       </c>
       <c r="AA41">
         <f t="shared" ca="1" si="11"/>
-        <v>0.84941000000000066</v>
+        <v>0.71264500000000019</v>
       </c>
       <c r="AB41">
         <f t="shared" ca="1" si="11"/>
-        <v>0.47883300000000162</v>
+        <v>0.34206800000000115</v>
       </c>
       <c r="AC41">
         <f t="shared" ca="1" si="11"/>
-        <v>1.4116550000000014</v>
+        <v>1.274890000000001</v>
       </c>
       <c r="AD41">
         <f t="shared" ca="1" si="11"/>
-        <v>0.36326200000000064</v>
+        <v>0.22649700000000017</v>
       </c>
       <c r="AE41">
         <f t="shared" ca="1" si="11"/>
-        <v>0.67846700000000126</v>
+        <v>0.54170200000000079</v>
       </c>
       <c r="AF41">
         <f t="shared" ca="1" si="11"/>
-        <v>0.51726300000000158</v>
+        <v>0.38049800000000111</v>
       </c>
       <c r="AG41">
         <f t="shared" ca="1" si="11"/>
-        <v>2.2469180000000009</v>
+        <v>2.1101530000000004</v>
       </c>
       <c r="AH41">
         <f t="shared" ca="1" si="11"/>
-        <v>1.3470290000000009</v>
+        <v>1.2102640000000005</v>
       </c>
       <c r="AI41">
         <f t="shared" ca="1" si="11"/>
-        <v>3.876297000000001</v>
+        <v>3.7395320000000005</v>
       </c>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.2">
@@ -9192,107 +9208,107 @@
       </c>
       <c r="B42">
         <f ca="1">SUM(B30:B41)</f>
-        <v>28.159041999999996</v>
+        <v>21.488436</v>
       </c>
       <c r="C42">
         <f ca="1">SUM(C30:C41)</f>
-        <v>20.136662000000001</v>
+        <v>13.156244000000004</v>
       </c>
       <c r="D42">
         <f ca="1">SUM(D30:D41)</f>
-        <v>20.722719999999995</v>
+        <v>17.584412</v>
       </c>
       <c r="E42">
         <f ca="1">SUM(E30:E41)</f>
-        <v>19.755296999999999</v>
+        <v>14.218850999999999</v>
       </c>
       <c r="F42">
         <f ca="1">SUM(F30:F41)</f>
-        <v>22.776882999999998</v>
+        <v>16.608831000000002</v>
       </c>
       <c r="L42">
         <f t="shared" ref="L42:V42" ca="1" si="12">SUM(L30:L41)</f>
-        <v>16.815100000000001</v>
+        <v>16.571647999999996</v>
       </c>
       <c r="M42">
         <f t="shared" ca="1" si="12"/>
-        <v>20.188502999999997</v>
+        <v>18.767209000000001</v>
       </c>
       <c r="N42">
         <f t="shared" ca="1" si="12"/>
-        <v>19.655194000000002</v>
+        <v>15.334393999999996</v>
       </c>
       <c r="O42">
         <f t="shared" ca="1" si="12"/>
-        <v>19.301707</v>
+        <v>15.952227000000002</v>
       </c>
       <c r="P42">
         <f t="shared" ca="1" si="12"/>
-        <v>16.574966000000003</v>
+        <v>20.396650000000001</v>
       </c>
       <c r="Q42">
         <f t="shared" ca="1" si="12"/>
-        <v>36.580233000000007</v>
+        <v>36.341465000000007</v>
       </c>
       <c r="R42">
         <f t="shared" ca="1" si="12"/>
-        <v>36.548141000000001</v>
+        <v>39.245086999999998</v>
       </c>
       <c r="S42">
         <f t="shared" ca="1" si="12"/>
-        <v>28.382021000000002</v>
+        <v>31.095146999999997</v>
       </c>
       <c r="T42">
         <f t="shared" ca="1" si="12"/>
-        <v>32.969042999999999</v>
+        <v>35.341977</v>
       </c>
       <c r="U42">
         <f t="shared" ca="1" si="12"/>
-        <v>40.368116000000001</v>
+        <v>42.470273999999996</v>
       </c>
       <c r="V42">
         <f t="shared" ca="1" si="12"/>
-        <v>107.047956</v>
+        <v>103.946774</v>
       </c>
       <c r="Z42">
         <f t="shared" ref="Z42:AI42" ca="1" si="13">SUM(Z30:Z41)</f>
-        <v>73.629621</v>
+        <v>69.871986000000007</v>
       </c>
       <c r="AA42">
         <f t="shared" ca="1" si="13"/>
-        <v>14.204040000000003</v>
+        <v>14.961130000000001</v>
       </c>
       <c r="AB42">
         <f t="shared" ca="1" si="13"/>
-        <v>14.558649000000003</v>
+        <v>14.051962999999997</v>
       </c>
       <c r="AC42">
         <f t="shared" ca="1" si="13"/>
-        <v>13.249385000000004</v>
+        <v>16.402601000000001</v>
       </c>
       <c r="AD42">
         <f t="shared" ca="1" si="13"/>
-        <v>12.908771</v>
+        <v>13.918888999999998</v>
       </c>
       <c r="AE42">
         <f t="shared" ca="1" si="13"/>
-        <v>12.263252999999999</v>
-      </c>
-      <c r="AF42">
+        <v>13.772168999999998</v>
+      </c>
+      <c r="AF42" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>15.217351999999998</v>
-      </c>
-      <c r="AG42">
+        <v>12.075807999999999</v>
+      </c>
+      <c r="AG42" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>12.540650999999997</v>
-      </c>
-      <c r="AH42">
+        <v>12.614428999999998</v>
+      </c>
+      <c r="AH42" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>10.094122000000002</v>
+        <v>11.983156000000005</v>
       </c>
       <c r="AI42">
         <f t="shared" ca="1" si="13"/>
-        <v>17.215086999999997</v>
+        <v>14.394327000000001</v>
       </c>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.2">
@@ -9302,31 +9318,31 @@
       </c>
       <c r="C43">
         <f ca="1">RANK(C42,$B$42:$AI$42,1)</f>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D43">
         <f ca="1">RANK(D42,$B$42:$AI$42,1)</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E43">
         <f ca="1">RANK(E42,$B$42:$AI$42,1)</f>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F43">
         <f ca="1">RANK(F42,$B$42:$AI$42,1)</f>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="L43">
         <f t="shared" ref="L43:V43" ca="1" si="14">RANK(L42,$B$42:$AI$42,1)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="M43">
         <f t="shared" ca="1" si="14"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N43">
         <f t="shared" ca="1" si="14"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="O43">
         <f t="shared" ca="1" si="14"/>
@@ -9334,15 +9350,15 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="14"/>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="Q43">
         <f t="shared" ca="1" si="14"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R43">
         <f t="shared" ca="1" si="14"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="S43">
         <f t="shared" ca="1" si="14"/>
@@ -9366,7 +9382,7 @@
       </c>
       <c r="AA43">
         <f t="shared" ca="1" si="15"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AB43">
         <f t="shared" ca="1" si="15"/>
@@ -9374,19 +9390,19 @@
       </c>
       <c r="AC43">
         <f t="shared" ca="1" si="15"/>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="AD43">
         <f t="shared" ca="1" si="15"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AE43">
         <f t="shared" ca="1" si="15"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AF43">
         <f t="shared" ca="1" si="15"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AG43">
         <f t="shared" ca="1" si="15"/>
@@ -9398,7 +9414,7 @@
       </c>
       <c r="AI43">
         <f t="shared" ca="1" si="15"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.2">
@@ -9407,107 +9423,107 @@
       </c>
       <c r="B44">
         <f ca="1">AVERAGE(B30:B41)</f>
-        <v>2.3465868333333328</v>
+        <v>1.7907029999999999</v>
       </c>
       <c r="C44">
         <f ca="1">AVERAGE(C30:C41)</f>
-        <v>1.6780551666666668</v>
+        <v>1.0963536666666671</v>
       </c>
       <c r="D44">
         <f ca="1">AVERAGE(D30:D41)</f>
-        <v>1.7268933333333329</v>
+        <v>1.4653676666666666</v>
       </c>
       <c r="E44">
         <f ca="1">AVERAGE(E30:E41)</f>
-        <v>1.6462747499999999</v>
+        <v>1.18490425</v>
       </c>
       <c r="F44">
         <f ca="1">AVERAGE(F30:F41)</f>
-        <v>1.8980735833333331</v>
+        <v>1.3840692500000003</v>
       </c>
       <c r="L44">
         <f t="shared" ref="L44:V44" ca="1" si="16">AVERAGE(L30:L41)</f>
-        <v>1.4012583333333335</v>
+        <v>1.3809706666666663</v>
       </c>
       <c r="M44">
         <f t="shared" ca="1" si="16"/>
-        <v>1.6823752499999998</v>
+        <v>1.5639340833333335</v>
       </c>
       <c r="N44">
         <f t="shared" ca="1" si="16"/>
-        <v>1.6379328333333334</v>
+        <v>1.2778661666666664</v>
       </c>
       <c r="O44">
         <f t="shared" ca="1" si="16"/>
-        <v>1.6084755833333333</v>
+        <v>1.3293522500000001</v>
       </c>
       <c r="P44">
         <f t="shared" ca="1" si="16"/>
-        <v>1.381247166666667</v>
+        <v>1.6997208333333333</v>
       </c>
       <c r="Q44">
         <f t="shared" ca="1" si="16"/>
-        <v>3.0483527500000007</v>
+        <v>3.0284554166666671</v>
       </c>
       <c r="R44">
         <f t="shared" ca="1" si="16"/>
-        <v>3.0456784166666666</v>
+        <v>3.2704239166666667</v>
       </c>
       <c r="S44">
         <f t="shared" ca="1" si="16"/>
-        <v>2.3651684166666667</v>
+        <v>2.5912622499999998</v>
       </c>
       <c r="T44">
         <f t="shared" ca="1" si="16"/>
-        <v>2.7474202499999998</v>
+        <v>2.94516475</v>
       </c>
       <c r="U44">
         <f t="shared" ca="1" si="16"/>
-        <v>3.3640096666666666</v>
+        <v>3.5391894999999995</v>
       </c>
       <c r="V44">
         <f t="shared" ca="1" si="16"/>
-        <v>8.9206629999999993</v>
+        <v>8.6622311666666665</v>
       </c>
       <c r="Z44">
         <f t="shared" ref="Z44:AI44" ca="1" si="17">AVERAGE(Z30:Z41)</f>
-        <v>6.6936019090909094</v>
+        <v>6.3519987272727283</v>
       </c>
       <c r="AA44">
         <f t="shared" ca="1" si="17"/>
-        <v>1.1836700000000002</v>
+        <v>1.2467608333333333</v>
       </c>
       <c r="AB44">
         <f t="shared" ca="1" si="17"/>
-        <v>1.2132207500000003</v>
+        <v>1.1709969166666665</v>
       </c>
       <c r="AC44">
         <f t="shared" ca="1" si="17"/>
-        <v>1.1041154166666669</v>
+        <v>1.3668834166666668</v>
       </c>
       <c r="AD44">
         <f t="shared" ca="1" si="17"/>
-        <v>1.0757309166666666</v>
+        <v>1.1599074166666665</v>
       </c>
       <c r="AE44">
         <f t="shared" ca="1" si="17"/>
-        <v>1.02193775</v>
-      </c>
-      <c r="AF44">
+        <v>1.1476807499999999</v>
+      </c>
+      <c r="AF44" s="2">
         <f t="shared" ca="1" si="17"/>
-        <v>1.2681126666666664</v>
-      </c>
-      <c r="AG44">
+        <v>1.0063173333333333</v>
+      </c>
+      <c r="AG44" s="2">
         <f t="shared" ca="1" si="17"/>
-        <v>1.0450542499999997</v>
-      </c>
-      <c r="AH44">
+        <v>1.0512024166666665</v>
+      </c>
+      <c r="AH44" s="2">
         <f t="shared" ca="1" si="17"/>
-        <v>0.84117683333333348</v>
+        <v>0.99859633333333375</v>
       </c>
       <c r="AI44">
         <f t="shared" ca="1" si="17"/>
-        <v>1.434590583333333</v>
+        <v>1.19952725</v>
       </c>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.2">
@@ -9517,31 +9533,31 @@
       </c>
       <c r="C45">
         <f ca="1">RANK(C44,$B$44:$AI$44,1)</f>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D45">
         <f ca="1">RANK(D44,$B$44:$AI$44,1)</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E45">
         <f ca="1">RANK(E44,$B$44:$AI$44,1)</f>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F45">
         <f ca="1">RANK(F44,$B$44:$AI$44,1)</f>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="L45">
         <f ca="1">RANK(L44,$B$44:$AI$44,1)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="M45">
         <f t="shared" ref="M45:AI45" ca="1" si="18">RANK(M44,$B$44:$AI$44,1)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N45">
         <f t="shared" ca="1" si="18"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="O45">
         <f t="shared" ca="1" si="18"/>
@@ -9549,15 +9565,15 @@
       </c>
       <c r="P45">
         <f t="shared" ca="1" si="18"/>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="Q45">
         <f t="shared" ca="1" si="18"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R45">
         <f t="shared" ca="1" si="18"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="S45">
         <f t="shared" ca="1" si="18"/>
@@ -9593,7 +9609,7 @@
       </c>
       <c r="AA45">
         <f t="shared" ca="1" si="18"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AB45">
         <f t="shared" ca="1" si="18"/>
@@ -9601,19 +9617,19 @@
       </c>
       <c r="AC45">
         <f t="shared" ca="1" si="18"/>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="AD45">
         <f t="shared" ca="1" si="18"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AE45">
         <f t="shared" ca="1" si="18"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AF45">
         <f t="shared" ca="1" si="18"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AG45">
         <f t="shared" ca="1" si="18"/>
@@ -9625,7 +9641,7 @@
       </c>
       <c r="AI45">
         <f t="shared" ca="1" si="18"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>